<commit_message>
Kleine Änderung an der Aufgabe
Hab nur bei einer Entity zwei Attribute vergessen.
</commit_message>
<xml_diff>
--- a/Aufgaben.xlsx
+++ b/Aufgaben.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/772e85f18d37e82d/Zeug/FH-Ordner/Stoff/Semester4/Web_Application_Development/QuizIt/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/772e85f18d37e82d/Zeug/FH-Ordner/Stoff/Semester4/Web_Application_Development/QuizIt/Repo/QuizIt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="208" documentId="8_{80271D84-3D5F-4BB3-9570-47F6BB9229E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00BD493E-BDE2-4784-91B0-0A399E02975B}"/>
+  <xr:revisionPtr revIDLastSave="209" documentId="8_{80271D84-3D5F-4BB3-9570-47F6BB9229E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2196E176-0E97-479F-A77A-B079CBB961BE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{766FD891-8964-469D-97C2-7D6F57F06240}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
-    <t>Erstelle Entity Settings (isPremiumUser, wantsMusic , wantsSportLeisure, wantsFilmTv, wantsArtsLiterature, wantsHistory, SocietyCulture, wantsScience, wantsGeography, wantsFoodDrink, wantsGeneralKnowledge)</t>
-  </si>
-  <si>
     <t>Erstelle Controller Function (User) deleteUser</t>
   </si>
   <si>
@@ -150,6 +147,9 @@
   </si>
   <si>
     <t>Minuten Pro Person:</t>
+  </si>
+  <si>
+    <t>Erstelle Entity Settings (id, userId, isPremiumUser, wantsMusic , wantsSportLeisure, wantsFilmTv, wantsArtsLiterature, wantsHistory, SocietyCulture, wantsScience, wantsGeography, wantsFoodDrink, wantsGeneralKnowledge)</t>
   </si>
 </sst>
 </file>
@@ -397,7 +397,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -753,7 +753,7 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,28 +765,28 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="C1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>19</v>
-      </c>
       <c r="H1" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -803,12 +803,12 @@
       <c r="D2" s="7"/>
       <c r="E2" s="8"/>
       <c r="F2" s="12">
-        <f>AVERAGE(B2:E2)</f>
+        <f t="shared" ref="F2:F30" si="0">AVERAGE(B2:E2)</f>
         <v>25</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -822,12 +822,12 @@
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="12">
-        <f>AVERAGE(B3:E3)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -841,12 +841,12 @@
       <c r="D4" s="9"/>
       <c r="E4" s="10"/>
       <c r="F4" s="12">
-        <f>AVERAGE(B4:E4)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="G4" s="15"/>
       <c r="H4" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -860,12 +860,12 @@
       <c r="D5" s="9"/>
       <c r="E5" s="10"/>
       <c r="F5" s="12">
-        <f>AVERAGE(B5:E5)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -879,12 +879,12 @@
       <c r="D6" s="9"/>
       <c r="E6" s="10"/>
       <c r="F6" s="12">
-        <f>AVERAGE(B6:E6)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="G6" s="15"/>
       <c r="H6" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -898,12 +898,12 @@
       <c r="D7" s="9"/>
       <c r="E7" s="10"/>
       <c r="F7" s="12">
-        <f>AVERAGE(B7:E7)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -917,12 +917,12 @@
       <c r="D8" s="9"/>
       <c r="E8" s="10"/>
       <c r="F8" s="12">
-        <f>AVERAGE(B8:E8)</f>
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="G8" s="15"/>
       <c r="H8" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -936,12 +936,12 @@
       <c r="D9" s="9"/>
       <c r="E9" s="10"/>
       <c r="F9" s="12">
-        <f>AVERAGE(B9:E9)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="G9" s="15"/>
       <c r="H9" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -955,12 +955,12 @@
       <c r="D10" s="9"/>
       <c r="E10" s="10"/>
       <c r="F10" s="12">
-        <f>AVERAGE(B10:E10)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -974,12 +974,12 @@
       <c r="D11" s="9"/>
       <c r="E11" s="10"/>
       <c r="F11" s="12">
-        <f>AVERAGE(B11:E11)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="G11" s="15"/>
       <c r="H11" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -993,12 +993,12 @@
       <c r="D12" s="9"/>
       <c r="E12" s="10"/>
       <c r="F12" s="12">
-        <f>AVERAGE(B12:E12)</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1012,12 +1012,12 @@
       <c r="D13" s="9"/>
       <c r="E13" s="10"/>
       <c r="F13" s="12">
-        <f>AVERAGE(B13:E13)</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="G13" s="15"/>
       <c r="H13" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1031,12 +1031,12 @@
       <c r="D14" s="9"/>
       <c r="E14" s="10"/>
       <c r="F14" s="12">
-        <f>AVERAGE(B14:E14)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="G14" s="15"/>
       <c r="H14" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1050,12 +1050,12 @@
       <c r="D15" s="9"/>
       <c r="E15" s="10"/>
       <c r="F15" s="12">
-        <f>AVERAGE(B15:E15)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1069,12 +1069,12 @@
       <c r="D16" s="9"/>
       <c r="E16" s="10"/>
       <c r="F16" s="12">
-        <f>AVERAGE(B16:E16)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G16" s="15"/>
       <c r="H16" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1088,12 +1088,12 @@
       <c r="D17" s="9"/>
       <c r="E17" s="10"/>
       <c r="F17" s="12">
-        <f>AVERAGE(B17:E17)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G17" s="15"/>
       <c r="H17" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1107,12 +1107,12 @@
       <c r="D18" s="9"/>
       <c r="E18" s="10"/>
       <c r="F18" s="12">
-        <f>AVERAGE(B18:E18)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G18" s="15"/>
       <c r="H18" s="4" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1126,12 +1126,12 @@
       <c r="D19" s="9"/>
       <c r="E19" s="10"/>
       <c r="F19" s="12">
-        <f>AVERAGE(B19:E19)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G19" s="15"/>
       <c r="H19" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1145,12 +1145,12 @@
       <c r="D20" s="9"/>
       <c r="E20" s="10"/>
       <c r="F20" s="12">
-        <f>AVERAGE(B20:E20)</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="G20" s="15"/>
       <c r="H20" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1164,12 +1164,12 @@
       <c r="D21" s="9"/>
       <c r="E21" s="10"/>
       <c r="F21" s="12">
-        <f>AVERAGE(B21:E21)</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="G21" s="15"/>
       <c r="H21" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1183,12 +1183,12 @@
       <c r="D22" s="9"/>
       <c r="E22" s="10"/>
       <c r="F22" s="12">
-        <f>AVERAGE(B22:E22)</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="G22" s="15"/>
       <c r="H22" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1202,12 +1202,12 @@
       <c r="D23" s="9"/>
       <c r="E23" s="10"/>
       <c r="F23" s="12">
-        <f>AVERAGE(B23:E23)</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="G23" s="15"/>
       <c r="H23" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1221,12 +1221,12 @@
       <c r="D24" s="9"/>
       <c r="E24" s="10"/>
       <c r="F24" s="12">
-        <f>AVERAGE(B24:E24)</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="G24" s="15"/>
       <c r="H24" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1240,12 +1240,12 @@
       <c r="D25" s="9"/>
       <c r="E25" s="10"/>
       <c r="F25" s="12">
-        <f>AVERAGE(B25:E25)</f>
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="G25" s="15"/>
       <c r="H25" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1259,12 +1259,12 @@
       <c r="D26" s="9"/>
       <c r="E26" s="10"/>
       <c r="F26" s="12">
-        <f>AVERAGE(B26:E26)</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="G26" s="15"/>
       <c r="H26" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1278,12 +1278,12 @@
       <c r="D27" s="9"/>
       <c r="E27" s="10"/>
       <c r="F27" s="12">
-        <f>AVERAGE(B27:E27)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="G27" s="15"/>
       <c r="H27" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1297,12 +1297,12 @@
       <c r="D28" s="9"/>
       <c r="E28" s="10"/>
       <c r="F28" s="12">
-        <f>AVERAGE(B28:E28)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="G28" s="15"/>
       <c r="H28" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1316,12 +1316,12 @@
       <c r="D29" s="9"/>
       <c r="E29" s="10"/>
       <c r="F29" s="12">
-        <f>AVERAGE(B29:E29)</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="G29" s="15"/>
       <c r="H29" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1335,12 +1335,12 @@
       <c r="D30" s="9"/>
       <c r="E30" s="10"/>
       <c r="F30" s="12">
-        <f>AVERAGE(B30:E30)</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="G30" s="15"/>
       <c r="H30" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1389,7 +1389,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E35" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F35" s="24">
         <f>SUM(F2:F34)/4</f>

</xml_diff>